<commit_message>
Creation of model at the end of the 2. day.
</commit_message>
<xml_diff>
--- a/VT_SHR_SUP_V01.xlsx
+++ b/VT_SHR_SUP_V01.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901" activeTab="1"/>
+    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
     <sheet name="SEC_Processes" sheetId="127" r:id="rId2"/>
     <sheet name="ProcessCharac_Horizontal" sheetId="131" r:id="rId3"/>
     <sheet name="EmissionTable" sheetId="126" r:id="rId4"/>
+    <sheet name="Demand" sheetId="132" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
@@ -1248,9 +1249,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="201" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1258,6 +1259,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1318,12 +1320,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="53"/>
       <name val="Arial"/>
@@ -1338,28 +1334,8 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -1506,7 +1482,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1520,8 +1496,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1533,7 +1509,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -1560,35 +1536,35 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="19" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="201" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="201" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="15" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="201" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
@@ -2459,7 +2435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
@@ -3775,4 +3751,18 @@
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Uranium added: the commodity and the import / export processes
</commit_message>
<xml_diff>
--- a/VT_SHR_SUP_V01.xlsx
+++ b/VT_SHR_SUP_V01.xlsx
@@ -5,16 +5,16 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mikkel Simonsen\TIMES-DK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Najub\TIMES-Shire\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901"/>
+    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
-    <sheet name="SEC_Processes" sheetId="127" r:id="rId2"/>
-    <sheet name="ProcessCharac_Horizontal" sheetId="131" r:id="rId3"/>
+    <sheet name="ProcessCharac_Horizontal" sheetId="131" r:id="rId2"/>
+    <sheet name="SEC_Processes" sheetId="127" r:id="rId3"/>
     <sheet name="EmissionTable" sheetId="126" r:id="rId4"/>
     <sheet name="Demand" sheetId="132" r:id="rId5"/>
   </sheets>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -343,10 +343,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Maurizio Gargiulo</author>
-    <author>Amit Kanudia</author>
   </authors>
   <commentList>
-    <comment ref="H7" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -355,418 +354,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Allowed TsLvl
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ANNUAL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Annual level)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>SEASON</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Seasonal level)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>WEEKLY</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Weekly level)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DAYNITE</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (day and night level)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I7" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Amit Kanudia:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Needed only when one wants to override the VEDA default assignment
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allowed Vintage</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-NO</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (if empty by default mean </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>NO</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-YES</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Sets declarations are </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>inherited. 
-Allowed Process Sets</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-ELE </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Thermal Electric Power Plant)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-CHP </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Combined Heat and Power)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-STGTSS </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Pump Storage)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-STGIPS</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Pump Storage IP)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-PRE </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Genric Process/Technology)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-DMD</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Demand Device)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-IMP </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">(Import)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>EXP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Export)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-MIN </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Mining Process)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-RNW </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Renewable Technology)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-HPL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Heating Plant)</t>
+          <t>With this character *, this column is ignored from VEDA.
+It is just useful for your information</t>
         </r>
       </text>
     </comment>
@@ -778,9 +367,10 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Maurizio Gargiulo</author>
+    <author>Amit Kanudia</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="H7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -789,8 +379,418 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>With this character *, this column is ignored from VEDA.
-It is just useful for your information</t>
+          <t xml:space="preserve">Allowed TsLvl
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ANNUAL</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (Annual level)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SEASON</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (Seasonal level)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>WEEKLY</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (Weekly level)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DAYNITE</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (day and night level)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amit Kanudia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Needed only when one wants to override the VEDA default assignment
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Allowed Vintage</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+NO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (if empty by default mean </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+YES</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Sets declarations are </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>inherited. 
+Allowed Process Sets</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ELE </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Thermal Electric Power Plant)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+CHP </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Combined Heat and Power)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+STGTSS </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Pump Storage)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+STGIPS</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (Pump Storage IP)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+PRE </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Genric Process/Technology)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+DMD</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (Demand Device)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+IMP </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">(Import)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>EXP</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (Export)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+MIN </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Mining Process)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RNW </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Renewable Technology)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HPL</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (Heating Plant)</t>
         </r>
       </text>
     </comment>
@@ -1572,7 +1572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="171">
   <si>
     <t>CommName</t>
   </si>
@@ -2042,9 +2042,6 @@
     <t>CRD, DSL, NGA</t>
   </si>
   <si>
-    <t>WIN, HYD, SOL</t>
-  </si>
-  <si>
     <t>HEAT</t>
   </si>
   <si>
@@ -2070,12 +2067,30 @@
   </si>
   <si>
     <t>ELC</t>
+  </si>
+  <si>
+    <t>URN</t>
+  </si>
+  <si>
+    <t>Uranium</t>
+  </si>
+  <si>
+    <t>IMPURN</t>
+  </si>
+  <si>
+    <t>Import Uranium</t>
+  </si>
+  <si>
+    <t>EXPURN</t>
+  </si>
+  <si>
+    <t>Export Uranium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
@@ -2319,7 +2334,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2420,6 +2435,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2930,25 +2946,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:J22"/>
+  <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2957,13 +2973,13 @@
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B6" s="33" t="s">
         <v>42</v>
       </c>
@@ -2976,7 +2992,7 @@
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36" t="s">
         <v>14</v>
       </c>
@@ -2989,7 +3005,7 @@
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="37" t="s">
         <v>7</v>
       </c>
@@ -3018,7 +3034,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="40" t="s">
         <v>47</v>
       </c>
@@ -3047,7 +3063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
         <v>58</v>
       </c>
@@ -3066,7 +3082,7 @@
       <c r="I10" s="42"/>
       <c r="J10" s="42"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
@@ -3083,7 +3099,7 @@
       <c r="I11" s="42"/>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
       <c r="D12" s="42" t="s">
@@ -3100,7 +3116,7 @@
       <c r="I12" s="42"/>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42" t="s">
@@ -3117,7 +3133,7 @@
       <c r="I13" s="42"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
       <c r="D14" s="42" t="s">
@@ -3134,7 +3150,7 @@
       <c r="I14" s="42"/>
       <c r="J14" s="42"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="s">
@@ -3151,7 +3167,7 @@
       <c r="I15" s="42"/>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
       <c r="D16" s="42" t="s">
@@ -3168,11 +3184,11 @@
       <c r="I16" s="42"/>
       <c r="J16" s="42"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
       <c r="D17" s="55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>94</v>
@@ -3185,7 +3201,7 @@
       <c r="I17" s="42"/>
       <c r="J17" s="42"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
@@ -3202,7 +3218,7 @@
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="42"/>
       <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
@@ -3219,52 +3235,52 @@
       <c r="I19" s="42"/>
       <c r="J19" s="42"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="42" t="s">
-        <v>63</v>
-      </c>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="42"/>
       <c r="C20" s="43"/>
-      <c r="D20" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>64</v>
+      <c r="D20" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="G20" s="42"/>
       <c r="H20" s="42"/>
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="43" t="s">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="43"/>
       <c r="C22" s="43"/>
       <c r="D22" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F22" s="43" t="s">
         <v>59</v>
@@ -3272,8 +3288,25 @@
       <c r="G22" s="43"/>
       <c r="H22" s="43"/>
       <c r="I22" s="43"/>
-      <c r="J22" s="55" t="s">
-        <v>165</v>
+      <c r="J22" s="43"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="55" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3287,489 +3320,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:M65533"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="7" style="15" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.88671875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" style="15" customWidth="1"/>
+    <col min="11" max="50" width="6" style="15" customWidth="1"/>
+    <col min="51" max="51" width="9.109375" style="15"/>
+    <col min="52" max="52" width="12" style="15" customWidth="1"/>
+    <col min="53" max="16384" width="9.109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B1" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-    </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="55" t="s">
-        <v>163</v>
-      </c>
-      <c r="E13" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="42" t="str">
-        <f>ProcessCharac_Horizontal!B27</f>
-        <v>EXPCOA</v>
-      </c>
-      <c r="E15" s="42" t="str">
-        <f>ProcessCharac_Horizontal!C27</f>
-        <v>Export Coal</v>
-      </c>
-      <c r="F15" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="55" t="s">
-        <v>164</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="F24" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42" t="str">
-        <f>ProcessCharac_Horizontal!B21</f>
-        <v>IMPCOA</v>
-      </c>
-      <c r="E25" s="42" t="str">
-        <f>ProcessCharac_Horizontal!C21</f>
-        <v>Import Coal</v>
-      </c>
-      <c r="F25" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65532"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="7" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.85546875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="15" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="15" customWidth="1"/>
-    <col min="11" max="50" width="6" style="15" customWidth="1"/>
-    <col min="51" max="51" width="9.140625" style="15"/>
-    <col min="52" max="52" width="12" style="15" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>56</v>
       </c>
@@ -3777,14 +3350,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="I2"/>
       <c r="J2" s="30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
@@ -3795,7 +3368,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I4" s="30" t="s">
         <v>78</v>
       </c>
@@ -3803,7 +3376,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
@@ -3816,7 +3389,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6"/>
@@ -3827,7 +3400,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -3838,7 +3411,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
@@ -3876,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="45" t="s">
         <v>49</v>
@@ -3911,7 +3484,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="46" t="s">
         <v>80</v>
@@ -3936,7 +3509,7 @@
       </c>
       <c r="M10" s="47"/>
     </row>
-    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="26" t="str">
         <f>SEC_Processes!D9</f>
@@ -3977,14 +3550,14 @@
       </c>
       <c r="M11" s="48"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
       <c r="B12" s="26" t="str">
-        <f>SEC_Processes!D16</f>
+        <f>SEC_Processes!D17</f>
         <v>IMPCRD</v>
       </c>
       <c r="C12" s="26" t="str">
-        <f>SEC_Processes!E16</f>
+        <f>SEC_Processes!E17</f>
         <v>Import Crude Oil</v>
       </c>
       <c r="D12" s="26"/>
@@ -4014,14 +3587,14 @@
       </c>
       <c r="M12" s="48"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="26" t="str">
-        <f>SEC_Processes!D17</f>
+        <f>SEC_Processes!D18</f>
         <v>IMPGSL</v>
       </c>
       <c r="C13" s="26" t="str">
-        <f>SEC_Processes!E17</f>
+        <f>SEC_Processes!E18</f>
         <v>Import Gasoline</v>
       </c>
       <c r="D13" s="26"/>
@@ -4049,14 +3622,14 @@
       </c>
       <c r="M13" s="48"/>
     </row>
-    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="26" t="str">
-        <f>SEC_Processes!D18</f>
+        <f>SEC_Processes!D19</f>
         <v>IMPWIN</v>
       </c>
       <c r="C14" s="26" t="str">
-        <f>SEC_Processes!E18</f>
+        <f>SEC_Processes!E19</f>
         <v>Import Wind</v>
       </c>
       <c r="D14" s="26"/>
@@ -4082,14 +3655,14 @@
       </c>
       <c r="M14" s="48"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="26" t="str">
-        <f>SEC_Processes!D19</f>
+        <f>SEC_Processes!D20</f>
         <v>IMPNGA</v>
       </c>
       <c r="C15" s="26" t="str">
-        <f>SEC_Processes!E19</f>
+        <f>SEC_Processes!E20</f>
         <v>Import Natural Gas</v>
       </c>
       <c r="D15" s="26"/>
@@ -4115,14 +3688,14 @@
       </c>
       <c r="M15" s="48"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="26" t="str">
-        <f>SEC_Processes!D20</f>
+        <f>SEC_Processes!D21</f>
         <v>IMPDSL</v>
       </c>
       <c r="C16" s="26" t="str">
-        <f>SEC_Processes!E20</f>
+        <f>SEC_Processes!E21</f>
         <v>Import Diesel</v>
       </c>
       <c r="D16" s="26"/>
@@ -4148,14 +3721,14 @@
       </c>
       <c r="M16" s="48"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="26" t="str">
-        <f>SEC_Processes!D21</f>
+        <f>SEC_Processes!D22</f>
         <v>IMPHYD</v>
       </c>
       <c r="C17" s="26" t="str">
-        <f>SEC_Processes!E21</f>
+        <f>SEC_Processes!E22</f>
         <v>Import Hydro</v>
       </c>
       <c r="D17" s="26"/>
@@ -4181,14 +3754,14 @@
       </c>
       <c r="M17" s="48"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="26" t="str">
-        <f>SEC_Processes!D22</f>
+        <f>SEC_Processes!D23</f>
         <v>IMPSOL</v>
       </c>
       <c r="C18" s="26" t="str">
-        <f>SEC_Processes!E22</f>
+        <f>SEC_Processes!E23</f>
         <v>Import Solar</v>
       </c>
       <c r="D18" s="26"/>
@@ -4214,14 +3787,14 @@
       </c>
       <c r="M18" s="48"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="26" t="str">
-        <f>SEC_Processes!D23</f>
+        <f>SEC_Processes!D24</f>
         <v>IMPWCH</v>
       </c>
       <c r="C19" s="26" t="str">
-        <f>SEC_Processes!E23</f>
+        <f>SEC_Processes!E24</f>
         <v>Import Woodchips</v>
       </c>
       <c r="D19" s="26"/>
@@ -4248,14 +3821,14 @@
       </c>
       <c r="M19" s="48"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="26" t="str">
-        <f>SEC_Processes!D24</f>
+        <f>SEC_Processes!D25</f>
         <v>IMPSTR</v>
       </c>
       <c r="C20" s="26" t="str">
-        <f>SEC_Processes!E24</f>
+        <f>SEC_Processes!E25</f>
         <v>Import Straw</v>
       </c>
       <c r="D20" s="26"/>
@@ -4281,7 +3854,7 @@
       </c>
       <c r="M20" s="48"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="26" t="s">
         <v>128</v>
@@ -4314,58 +3887,49 @@
       </c>
       <c r="M21" s="48"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
-      <c r="B22" s="26" t="str">
+      <c r="B22" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="26"/>
+      <c r="E22" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="48">
+        <v>0.8</v>
+      </c>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48">
+        <v>0.81</v>
+      </c>
+      <c r="M22" s="48"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="26" t="str">
         <f>SEC_Processes!D10</f>
         <v>EXPCRD</v>
       </c>
-      <c r="C22" s="26" t="str">
+      <c r="C23" s="26" t="str">
         <f>SEC_Processes!E10</f>
         <v>Export Crude Oil</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D23" s="27" t="s">
         <v>60</v>
-      </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="I22" s="48">
-        <f>I12*$J$3</f>
-        <v>14.25</v>
-      </c>
-      <c r="J22" s="48">
-        <f>J12*$J$3</f>
-        <v>12.35</v>
-      </c>
-      <c r="K22" s="48">
-        <f>K12*$J$3</f>
-        <v>12.35</v>
-      </c>
-      <c r="L22" s="48">
-        <f>L12*$J$3</f>
-        <v>7.6</v>
-      </c>
-      <c r="M22" s="48"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B23" s="26" t="str">
-        <f>SEC_Processes!D11</f>
-        <v>EXPNGA</v>
-      </c>
-      <c r="C23" s="26" t="str">
-        <f>SEC_Processes!E11</f>
-        <v>Export Natural Gas</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>86</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="27" t="s">
@@ -4378,28 +3942,34 @@
         <v>79</v>
       </c>
       <c r="I23" s="48">
-        <f>I15*J3</f>
-        <v>9.234</v>
-      </c>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
+        <f>I12*$J$3</f>
+        <v>14.25</v>
+      </c>
+      <c r="J23" s="48">
+        <f>J12*$J$3</f>
+        <v>12.35</v>
+      </c>
+      <c r="K23" s="48">
+        <f>K12*$J$3</f>
+        <v>12.35</v>
+      </c>
       <c r="L23" s="48">
-        <f>L15*J3</f>
-        <v>8.5214999999999996</v>
+        <f>L12*$J$3</f>
+        <v>7.6</v>
       </c>
       <c r="M23" s="48"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="str">
-        <f>SEC_Processes!D12</f>
-        <v>EXPDSL</v>
+        <f>SEC_Processes!D11</f>
+        <v>EXPNGA</v>
       </c>
       <c r="C24" s="26" t="str">
-        <f>SEC_Processes!E12</f>
-        <v>Export Diesel</v>
+        <f>SEC_Processes!E11</f>
+        <v>Export Natural Gas</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="27" t="s">
@@ -4412,31 +3982,30 @@
         <v>79</v>
       </c>
       <c r="I24" s="48">
-        <f>I16*J3</f>
-        <v>19.579499999999999</v>
+        <f>I15*J3</f>
+        <v>9.234</v>
       </c>
       <c r="J24" s="48"/>
       <c r="K24" s="48"/>
       <c r="L24" s="48">
-        <f>L16*J3</f>
-        <v>13.433</v>
+        <f>L15*J3</f>
+        <v>8.5214999999999996</v>
       </c>
       <c r="M24" s="48"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="str">
-        <f>SEC_Processes!D13</f>
-        <v>EXPWCH</v>
+        <f>SEC_Processes!D12</f>
+        <v>EXPDSL</v>
       </c>
       <c r="C25" s="26" t="str">
-        <f>SEC_Processes!E13</f>
-        <v>Export Woodchips</v>
-      </c>
-      <c r="D25" s="26" t="str">
-        <f>SEC_Comm!D17</f>
-        <v>WCH</v>
-      </c>
-      <c r="E25" s="26"/>
+        <f>SEC_Processes!E12</f>
+        <v>Export Diesel</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="27"/>
       <c r="F25" s="27" t="s">
         <v>74</v>
       </c>
@@ -4447,28 +4016,29 @@
         <v>79</v>
       </c>
       <c r="I25" s="48">
-        <f>I19*J3</f>
-        <v>5.794999999999999</v>
+        <f>I16*J3</f>
+        <v>19.579499999999999</v>
       </c>
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
       <c r="L25" s="48">
-        <f>L19*J3</f>
-        <v>5.89</v>
+        <f>L16*J3</f>
+        <v>13.433</v>
       </c>
       <c r="M25" s="48"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="str">
-        <f>SEC_Processes!D14</f>
-        <v>EXPSTR</v>
+        <f>SEC_Processes!D13</f>
+        <v>EXPWCH</v>
       </c>
       <c r="C26" s="26" t="str">
-        <f>SEC_Processes!E14</f>
-        <v>Export Straw</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>95</v>
+        <f>SEC_Processes!E13</f>
+        <v>Export Woodchips</v>
+      </c>
+      <c r="D26" s="26" t="str">
+        <f>SEC_Comm!D17</f>
+        <v>WCH</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="27" t="s">
@@ -4481,26 +4051,28 @@
         <v>79</v>
       </c>
       <c r="I26" s="48">
-        <f>I20*J3</f>
-        <v>5.2249999999999996</v>
+        <f>I19*J3</f>
+        <v>5.794999999999999</v>
       </c>
       <c r="J26" s="48"/>
       <c r="K26" s="48"/>
       <c r="L26" s="48">
-        <f>L20*J3</f>
-        <v>5.3199999999999994</v>
+        <f>L19*J3</f>
+        <v>5.89</v>
       </c>
       <c r="M26" s="48"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B27" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>131</v>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="26" t="str">
+        <f>SEC_Processes!D14</f>
+        <v>EXPSTR</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>SEC_Processes!E14</f>
+        <v>Export Straw</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
@@ -4513,26 +4085,592 @@
         <v>79</v>
       </c>
       <c r="I27" s="48">
-        <f>I23*0.7</f>
-        <v>6.4638</v>
+        <f>I20*J3</f>
+        <v>5.2249999999999996</v>
       </c>
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
       <c r="L27" s="48">
-        <f>L23*0.7</f>
+        <f>L20*J3</f>
+        <v>5.3199999999999994</v>
+      </c>
+      <c r="M27" s="48"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28" s="48">
+        <f>I24*0.7</f>
+        <v>6.4638</v>
+      </c>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48">
+        <f>L24*0.7</f>
         <v>5.9650499999999997</v>
       </c>
-      <c r="M27" s="48"/>
-    </row>
-    <row r="65532" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F65532" s="27" t="s">
+      <c r="M28" s="48"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="48">
+        <f>I22*$J$3</f>
+        <v>0.76</v>
+      </c>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48">
+        <f>L22*$J$3</f>
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="M29" s="48"/>
+    </row>
+    <row r="65533" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F65533" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="G65532" s="27"/>
+      <c r="G65533" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292"/>
+  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B1" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+    </row>
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="42" t="str">
+        <f>ProcessCharac_Horizontal!B28</f>
+        <v>EXPCOA</v>
+      </c>
+      <c r="E15" s="42" t="str">
+        <f>ProcessCharac_Horizontal!C28</f>
+        <v>Export Coal</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="42" t="str">
+        <f>ProcessCharac_Horizontal!B29</f>
+        <v>EXPURN</v>
+      </c>
+      <c r="E16" s="42" t="str">
+        <f>ProcessCharac_Horizontal!C29</f>
+        <v>Export Uranium</v>
+      </c>
+      <c r="F16" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42" t="str">
+        <f>ProcessCharac_Horizontal!B21</f>
+        <v>IMPCOA</v>
+      </c>
+      <c r="E26" s="42" t="str">
+        <f>ProcessCharac_Horizontal!C21</f>
+        <v>Import Coal</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42" t="str">
+        <f>ProcessCharac_Horizontal!B22</f>
+        <v>IMPURN</v>
+      </c>
+      <c r="E27" s="42" t="str">
+        <f>ProcessCharac_Horizontal!C22</f>
+        <v>Import Uranium</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -4546,19 +4684,19 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -4567,7 +4705,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
@@ -4575,27 +4713,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
@@ -4611,29 +4749,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="49" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B5" s="51" t="s">
         <v>0</v>
       </c>
@@ -4647,7 +4785,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>138</v>
       </c>
@@ -4655,7 +4793,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>123</v>
       </c>
@@ -4663,7 +4801,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>122</v>
       </c>
@@ -4671,12 +4809,12 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
         <v>1</v>
       </c>
@@ -4703,7 +4841,7 @@
       </c>
       <c r="J14" s="38"/>
     </row>
-    <row r="15" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="41" t="s">
         <v>49</v>
       </c>
@@ -4730,7 +4868,7 @@
       </c>
       <c r="J15" s="41"/>
     </row>
-    <row r="16" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="46" t="s">
         <v>80</v>
       </c>
@@ -4747,7 +4885,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="43" t="s">
         <v>151</v>
       </c>
@@ -4761,7 +4899,7 @@
         <v>138</v>
       </c>
       <c r="F17" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G17" s="54">
         <v>1</v>
@@ -4772,7 +4910,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="43" t="s">
         <v>149</v>
       </c>
@@ -4780,13 +4918,13 @@
         <v>153</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="E18" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="43" t="s">
         <v>158</v>
-      </c>
-      <c r="F18" s="43" t="s">
-        <v>159</v>
       </c>
       <c r="G18" s="54">
         <v>1</v>
@@ -4797,7 +4935,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="43" t="s">
         <v>150</v>
       </c>
@@ -4808,10 +4946,10 @@
         <v>122</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F19" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G19" s="54">
         <v>1</v>
@@ -4822,7 +4960,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="36" t="s">
         <v>16</v>
       </c>
@@ -4835,7 +4973,7 @@
       <c r="I25" s="44"/>
       <c r="J25" s="44"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
         <v>11</v>
       </c>
@@ -4864,7 +5002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="41" t="s">
         <v>48</v>
       </c>
@@ -4893,9 +5031,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C28" s="43"/>
       <c r="D28" s="43" t="s">
@@ -4912,7 +5050,7 @@
       <c r="I28" s="54"/>
       <c r="J28" s="54"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="43"/>
       <c r="C29" s="43"/>
       <c r="D29" s="43" t="s">
@@ -4929,7 +5067,7 @@
       <c r="I29" s="54"/>
       <c r="J29" s="54"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
       <c r="D30" s="43" t="s">
@@ -4946,7 +5084,7 @@
       <c r="I30" s="54"/>
       <c r="J30" s="54"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="36" t="s">
         <v>14</v>
       </c>
@@ -4959,7 +5097,7 @@
       <c r="I32" s="35"/>
       <c r="J32" s="35"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="37" t="s">
         <v>7</v>
       </c>
@@ -4988,7 +5126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="40" t="s">
         <v>47</v>
       </c>
@@ -5017,13 +5155,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="43" t="s">
         <v>58</v>
       </c>
       <c r="C35" s="43"/>
       <c r="D35" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E35" s="43" t="s">
         <v>124</v>
@@ -5036,11 +5174,11 @@
       <c r="I35" s="43"/>
       <c r="J35" s="43"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
       <c r="D36" s="43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E36" s="43" t="s">
         <v>125</v>
@@ -5053,14 +5191,14 @@
       <c r="I36" s="43"/>
       <c r="J36" s="43"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="43"/>
       <c r="C37" s="43"/>
       <c r="D37" s="43" t="s">
         <v>138</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F37" s="43" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Uranium added and flag for ELCC was missing
</commit_message>
<xml_diff>
--- a/VT_SHR_SUP_V01.xlsx
+++ b/VT_SHR_SUP_V01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mikkel Simonsen\TIMES-DK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Najub\TIMES-Shire\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901" activeTab="1"/>
+    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -821,7 +821,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="147">
   <si>
     <t>CommName</t>
   </si>
@@ -1241,16 +1241,37 @@
   </si>
   <si>
     <t>Gasoline</t>
+  </si>
+  <si>
+    <t>URN</t>
+  </si>
+  <si>
+    <t>Uranium</t>
+  </si>
+  <si>
+    <t>IMPURN</t>
+  </si>
+  <si>
+    <t>Import Uranium</t>
+  </si>
+  <si>
+    <t>EXPURN</t>
+  </si>
+  <si>
+    <t>Export Uranium</t>
+  </si>
+  <si>
+    <t>ELC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="201" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1318,12 +1339,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="53"/>
       <name val="Arial"/>
@@ -1338,28 +1353,8 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -1506,7 +1501,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1520,8 +1515,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1533,7 +1528,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -1560,35 +1555,35 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="19" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="201" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="201" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="15" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="201" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
@@ -2102,25 +2097,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:J22"/>
+  <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:J25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2129,13 +2124,13 @@
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B6" s="33" t="s">
         <v>42</v>
       </c>
@@ -2148,7 +2143,7 @@
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36" t="s">
         <v>14</v>
       </c>
@@ -2161,7 +2156,7 @@
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="37" t="s">
         <v>7</v>
       </c>
@@ -2190,7 +2185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="40" t="s">
         <v>47</v>
       </c>
@@ -2219,7 +2214,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
         <v>58</v>
       </c>
@@ -2238,7 +2233,7 @@
       <c r="I10" s="42"/>
       <c r="J10" s="42"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
@@ -2255,7 +2250,7 @@
       <c r="I11" s="42"/>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
       <c r="D12" s="42" t="s">
@@ -2272,7 +2267,7 @@
       <c r="I12" s="42"/>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42" t="s">
@@ -2289,7 +2284,7 @@
       <c r="I13" s="42"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
       <c r="D14" s="42" t="s">
@@ -2306,7 +2301,7 @@
       <c r="I14" s="42"/>
       <c r="J14" s="42"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="s">
@@ -2323,7 +2318,7 @@
       <c r="I15" s="42"/>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
       <c r="D16" s="42" t="s">
@@ -2340,7 +2335,7 @@
       <c r="I16" s="42"/>
       <c r="J16" s="42"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
       <c r="D17" s="42" t="s">
@@ -2357,7 +2352,7 @@
       <c r="I17" s="42"/>
       <c r="J17" s="42"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
@@ -2374,7 +2369,7 @@
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="42"/>
       <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
@@ -2391,52 +2386,52 @@
       <c r="I19" s="42"/>
       <c r="J19" s="42"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="42" t="s">
-        <v>63</v>
-      </c>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="42"/>
       <c r="C20" s="43"/>
       <c r="D20" s="42" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G20" s="42"/>
       <c r="H20" s="42"/>
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="43" t="s">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="43"/>
       <c r="C22" s="43"/>
       <c r="D22" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F22" s="43" t="s">
         <v>59</v>
@@ -2445,6 +2440,25 @@
       <c r="H22" s="43"/>
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2457,38 +2471,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="33" t="s">
         <v>43</v>
@@ -2502,7 +2516,7 @@
       <c r="I5" s="44"/>
       <c r="J5" s="44"/>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
         <v>16</v>
       </c>
@@ -2515,7 +2529,7 @@
       <c r="I6" s="44"/>
       <c r="J6" s="44"/>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
         <v>11</v>
       </c>
@@ -2544,7 +2558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="41" t="s">
         <v>48</v>
       </c>
@@ -2573,7 +2587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="42" t="s">
         <v>68</v>
       </c>
@@ -2594,7 +2608,7 @@
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
         <v>70</v>
       </c>
@@ -2615,7 +2629,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
@@ -2634,7 +2648,7 @@
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="42"/>
       <c r="C12" s="43"/>
       <c r="D12" s="42" t="s">
@@ -2653,7 +2667,7 @@
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
       <c r="C13" s="43"/>
       <c r="D13" s="42" t="s">
@@ -2672,7 +2686,7 @@
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
       <c r="D14" s="42" t="s">
@@ -2691,15 +2705,15 @@
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="str">
-        <f>ProcessCharac_Horizontal!B27</f>
+        <f>ProcessCharac_Horizontal!B28</f>
         <v>EXPCOA</v>
       </c>
       <c r="E15" s="42" t="str">
-        <f>ProcessCharac_Horizontal!C27</f>
+        <f>ProcessCharac_Horizontal!C28</f>
         <v>Export Coal</v>
       </c>
       <c r="F15" s="42" t="s">
@@ -2712,16 +2726,16 @@
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="42" t="s">
-        <v>65</v>
-      </c>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="42"/>
       <c r="C16" s="43"/>
-      <c r="D16" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="42" t="s">
-        <v>117</v>
+      <c r="D16" s="42" t="str">
+        <f>ProcessCharac_Horizontal!B29</f>
+        <v>EXPURN</v>
+      </c>
+      <c r="E16" s="42" t="str">
+        <f>ProcessCharac_Horizontal!C29</f>
+        <v>Export Uranium</v>
       </c>
       <c r="F16" s="42" t="s">
         <v>59</v>
@@ -2733,14 +2747,16 @@
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="42"/>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
+        <v>65</v>
+      </c>
       <c r="C17" s="43"/>
       <c r="D17" s="42" t="s">
-        <v>136</v>
+        <v>66</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>59</v>
@@ -2752,14 +2768,14 @@
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="43"/>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="F18" s="42" t="s">
         <v>59</v>
@@ -2771,14 +2787,14 @@
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F19" s="42" t="s">
         <v>59</v>
@@ -2786,18 +2802,18 @@
       <c r="G19" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
       <c r="D20" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>59</v>
@@ -2809,14 +2825,14 @@
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F21" s="42" t="s">
         <v>59</v>
@@ -2828,14 +2844,14 @@
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
       <c r="D22" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F22" s="42" t="s">
         <v>59</v>
@@ -2847,14 +2863,14 @@
       <c r="I22" s="42"/>
       <c r="J22" s="42"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="42"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F23" s="42" t="s">
         <v>59</v>
@@ -2866,14 +2882,14 @@
       <c r="I23" s="42"/>
       <c r="J23" s="42"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="42"/>
       <c r="C24" s="42"/>
       <c r="D24" s="42" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F24" s="42" t="s">
         <v>59</v>
@@ -2885,16 +2901,14 @@
       <c r="I24" s="42"/>
       <c r="J24" s="42"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="42"/>
       <c r="C25" s="42"/>
-      <c r="D25" s="42" t="str">
-        <f>ProcessCharac_Horizontal!B21</f>
-        <v>IMPCOA</v>
-      </c>
-      <c r="E25" s="42" t="str">
-        <f>ProcessCharac_Horizontal!C21</f>
-        <v>Import Coal</v>
+      <c r="D25" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>116</v>
       </c>
       <c r="F25" s="42" t="s">
         <v>59</v>
@@ -2905,6 +2919,48 @@
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42" t="str">
+        <f>ProcessCharac_Horizontal!B21</f>
+        <v>IMPCOA</v>
+      </c>
+      <c r="E26" s="42" t="str">
+        <f>ProcessCharac_Horizontal!C21</f>
+        <v>Import Coal</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42" t="str">
+        <f>ProcessCharac_Horizontal!B22</f>
+        <v>IMPURN</v>
+      </c>
+      <c r="E27" s="42" t="str">
+        <f>ProcessCharac_Horizontal!C22</f>
+        <v>Import Uranium</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2917,29 +2973,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65532"/>
+  <dimension ref="A1:M65533"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.85546875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="15" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.88671875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" style="15" customWidth="1"/>
     <col min="11" max="50" width="6" style="15" customWidth="1"/>
-    <col min="51" max="51" width="9.140625" style="15"/>
+    <col min="51" max="51" width="9.109375" style="15"/>
     <col min="52" max="52" width="12" style="15" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="15"/>
+    <col min="53" max="16384" width="9.109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>56</v>
       </c>
@@ -2947,14 +3003,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="I2"/>
       <c r="J2" s="30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
@@ -2965,7 +3021,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I4" s="30" t="s">
         <v>78</v>
       </c>
@@ -2973,7 +3029,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
@@ -2986,7 +3042,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6"/>
@@ -2997,7 +3053,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -3008,7 +3064,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
@@ -3046,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="45" t="s">
         <v>49</v>
@@ -3081,7 +3137,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="46" t="s">
         <v>80</v>
@@ -3106,7 +3162,7 @@
       </c>
       <c r="M10" s="47"/>
     </row>
-    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="26" t="str">
         <f>SEC_Processes!D9</f>
@@ -3147,14 +3203,14 @@
       </c>
       <c r="M11" s="48"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
       <c r="B12" s="26" t="str">
-        <f>SEC_Processes!D16</f>
+        <f>SEC_Processes!D17</f>
         <v>IMPCRD</v>
       </c>
       <c r="C12" s="26" t="str">
-        <f>SEC_Processes!E16</f>
+        <f>SEC_Processes!E17</f>
         <v>Import Crude Oil</v>
       </c>
       <c r="D12" s="26"/>
@@ -3184,14 +3240,14 @@
       </c>
       <c r="M12" s="48"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="26" t="str">
-        <f>SEC_Processes!D17</f>
+        <f>SEC_Processes!D18</f>
         <v>IMPGSL</v>
       </c>
       <c r="C13" s="26" t="str">
-        <f>SEC_Processes!E17</f>
+        <f>SEC_Processes!E18</f>
         <v>Import Gasoline</v>
       </c>
       <c r="D13" s="26"/>
@@ -3219,14 +3275,14 @@
       </c>
       <c r="M13" s="48"/>
     </row>
-    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="26" t="str">
-        <f>SEC_Processes!D18</f>
+        <f>SEC_Processes!D19</f>
         <v>IMPWIN</v>
       </c>
       <c r="C14" s="26" t="str">
-        <f>SEC_Processes!E18</f>
+        <f>SEC_Processes!E19</f>
         <v>Import Wind</v>
       </c>
       <c r="D14" s="26"/>
@@ -3252,14 +3308,14 @@
       </c>
       <c r="M14" s="48"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="26" t="str">
-        <f>SEC_Processes!D19</f>
+        <f>SEC_Processes!D20</f>
         <v>IMPNGA</v>
       </c>
       <c r="C15" s="26" t="str">
-        <f>SEC_Processes!E19</f>
+        <f>SEC_Processes!E20</f>
         <v>Import Natural Gas</v>
       </c>
       <c r="D15" s="26"/>
@@ -3285,14 +3341,14 @@
       </c>
       <c r="M15" s="48"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="26" t="str">
-        <f>SEC_Processes!D20</f>
+        <f>SEC_Processes!D21</f>
         <v>IMPDSL</v>
       </c>
       <c r="C16" s="26" t="str">
-        <f>SEC_Processes!E20</f>
+        <f>SEC_Processes!E21</f>
         <v>Import Diesel</v>
       </c>
       <c r="D16" s="26"/>
@@ -3318,14 +3374,14 @@
       </c>
       <c r="M16" s="48"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="26" t="str">
-        <f>SEC_Processes!D21</f>
+        <f>SEC_Processes!D22</f>
         <v>IMPHYD</v>
       </c>
       <c r="C17" s="26" t="str">
-        <f>SEC_Processes!E21</f>
+        <f>SEC_Processes!E22</f>
         <v>Import Hydro</v>
       </c>
       <c r="D17" s="26"/>
@@ -3351,14 +3407,14 @@
       </c>
       <c r="M17" s="48"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="26" t="str">
-        <f>SEC_Processes!D22</f>
+        <f>SEC_Processes!D23</f>
         <v>IMPSOL</v>
       </c>
       <c r="C18" s="26" t="str">
-        <f>SEC_Processes!E22</f>
+        <f>SEC_Processes!E23</f>
         <v>Import Solar</v>
       </c>
       <c r="D18" s="26"/>
@@ -3384,14 +3440,14 @@
       </c>
       <c r="M18" s="48"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="26" t="str">
-        <f>SEC_Processes!D23</f>
+        <f>SEC_Processes!D24</f>
         <v>IMPWPE</v>
       </c>
       <c r="C19" s="26" t="str">
-        <f>SEC_Processes!E23</f>
+        <f>SEC_Processes!E24</f>
         <v>Import Woodchips</v>
       </c>
       <c r="D19" s="26"/>
@@ -3418,14 +3474,14 @@
       </c>
       <c r="M19" s="48"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="26" t="str">
-        <f>SEC_Processes!D24</f>
+        <f>SEC_Processes!D25</f>
         <v>IMPSTR</v>
       </c>
       <c r="C20" s="26" t="str">
-        <f>SEC_Processes!E24</f>
+        <f>SEC_Processes!E25</f>
         <v>Import Straw</v>
       </c>
       <c r="D20" s="26"/>
@@ -3451,7 +3507,7 @@
       </c>
       <c r="M20" s="48"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="26" t="s">
         <v>128</v>
@@ -3484,58 +3540,49 @@
       </c>
       <c r="M21" s="48"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
-      <c r="B22" s="26" t="str">
+      <c r="B22" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="48">
+        <v>0.8</v>
+      </c>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48">
+        <v>0.81</v>
+      </c>
+      <c r="M22" s="48"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="26" t="str">
         <f>SEC_Processes!D10</f>
         <v>EXPCRD</v>
       </c>
-      <c r="C22" s="26" t="str">
+      <c r="C23" s="26" t="str">
         <f>SEC_Processes!E10</f>
         <v>Export Crude Oil</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D23" s="27" t="s">
         <v>60</v>
-      </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="I22" s="48">
-        <f>I12*$J$3</f>
-        <v>14.25</v>
-      </c>
-      <c r="J22" s="48">
-        <f>J12*$J$3</f>
-        <v>12.35</v>
-      </c>
-      <c r="K22" s="48">
-        <f>K12*$J$3</f>
-        <v>12.35</v>
-      </c>
-      <c r="L22" s="48">
-        <f>L12*$J$3</f>
-        <v>7.6</v>
-      </c>
-      <c r="M22" s="48"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B23" s="26" t="str">
-        <f>SEC_Processes!D11</f>
-        <v>EXPNGA</v>
-      </c>
-      <c r="C23" s="26" t="str">
-        <f>SEC_Processes!E11</f>
-        <v>Export Natural Gas</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>86</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="27" t="s">
@@ -3548,28 +3595,34 @@
         <v>79</v>
       </c>
       <c r="I23" s="48">
-        <f>I15*J3</f>
-        <v>9.234</v>
-      </c>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
+        <f>I12*$J$3</f>
+        <v>14.25</v>
+      </c>
+      <c r="J23" s="48">
+        <f>J12*$J$3</f>
+        <v>12.35</v>
+      </c>
+      <c r="K23" s="48">
+        <f>K12*$J$3</f>
+        <v>12.35</v>
+      </c>
       <c r="L23" s="48">
-        <f>L15*J3</f>
-        <v>8.5214999999999996</v>
+        <f>L12*$J$3</f>
+        <v>7.6</v>
       </c>
       <c r="M23" s="48"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="str">
-        <f>SEC_Processes!D12</f>
-        <v>EXPDSL</v>
+        <f>SEC_Processes!D11</f>
+        <v>EXPNGA</v>
       </c>
       <c r="C24" s="26" t="str">
-        <f>SEC_Processes!E12</f>
-        <v>Export Diesel</v>
+        <f>SEC_Processes!E11</f>
+        <v>Export Natural Gas</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="27" t="s">
@@ -3582,31 +3635,30 @@
         <v>79</v>
       </c>
       <c r="I24" s="48">
-        <f>I16*J3</f>
-        <v>19.579499999999999</v>
+        <f>I15*J3</f>
+        <v>9.234</v>
       </c>
       <c r="J24" s="48"/>
       <c r="K24" s="48"/>
       <c r="L24" s="48">
-        <f>L16*J3</f>
-        <v>13.433</v>
+        <f>L15*J3</f>
+        <v>8.5214999999999996</v>
       </c>
       <c r="M24" s="48"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="str">
-        <f>SEC_Processes!D13</f>
-        <v>EXPWPE</v>
+        <f>SEC_Processes!D12</f>
+        <v>EXPDSL</v>
       </c>
       <c r="C25" s="26" t="str">
-        <f>SEC_Processes!E13</f>
-        <v>Export Woodchips</v>
-      </c>
-      <c r="D25" s="26" t="str">
-        <f>SEC_Comm!D17</f>
-        <v>WPE</v>
-      </c>
-      <c r="E25" s="26"/>
+        <f>SEC_Processes!E12</f>
+        <v>Export Diesel</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="27"/>
       <c r="F25" s="27" t="s">
         <v>74</v>
       </c>
@@ -3617,28 +3669,29 @@
         <v>79</v>
       </c>
       <c r="I25" s="48">
-        <f>I19*J3</f>
-        <v>5.794999999999999</v>
+        <f>I16*J3</f>
+        <v>19.579499999999999</v>
       </c>
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
       <c r="L25" s="48">
-        <f>L19*J3</f>
-        <v>5.89</v>
+        <f>L16*J3</f>
+        <v>13.433</v>
       </c>
       <c r="M25" s="48"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="str">
-        <f>SEC_Processes!D14</f>
-        <v>EXPSTR</v>
+        <f>SEC_Processes!D13</f>
+        <v>EXPWPE</v>
       </c>
       <c r="C26" s="26" t="str">
-        <f>SEC_Processes!E14</f>
-        <v>Export Straw</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>95</v>
+        <f>SEC_Processes!E13</f>
+        <v>Export Woodchips</v>
+      </c>
+      <c r="D26" s="26" t="str">
+        <f>SEC_Comm!D17</f>
+        <v>WPE</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="27" t="s">
@@ -3651,26 +3704,28 @@
         <v>79</v>
       </c>
       <c r="I26" s="48">
-        <f>I20*J3</f>
-        <v>5.2249999999999996</v>
+        <f>I19*J3</f>
+        <v>5.794999999999999</v>
       </c>
       <c r="J26" s="48"/>
       <c r="K26" s="48"/>
       <c r="L26" s="48">
-        <f>L20*J3</f>
-        <v>5.3199999999999994</v>
+        <f>L19*J3</f>
+        <v>5.89</v>
       </c>
       <c r="M26" s="48"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B27" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>131</v>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="26" t="str">
+        <f>SEC_Processes!D14</f>
+        <v>EXPSTR</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>SEC_Processes!E14</f>
+        <v>Export Straw</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
@@ -3683,22 +3738,86 @@
         <v>79</v>
       </c>
       <c r="I27" s="48">
-        <f>I23*0.7</f>
-        <v>6.4638</v>
+        <f>I20*J3</f>
+        <v>5.2249999999999996</v>
       </c>
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
       <c r="L27" s="48">
-        <f>L23*0.7</f>
+        <f>L20*J3</f>
+        <v>5.3199999999999994</v>
+      </c>
+      <c r="M27" s="48"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28" s="48">
+        <f>I24*0.7</f>
+        <v>6.4638</v>
+      </c>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48">
+        <f>L24*0.7</f>
         <v>5.9650499999999997</v>
       </c>
-      <c r="M27" s="48"/>
-    </row>
-    <row r="65532" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F65532" s="27" t="s">
+      <c r="M28" s="48"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="48">
+        <f>I22*$J$3</f>
+        <v>0.76</v>
+      </c>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48">
+        <f>L22*$J$3</f>
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="M29" s="48"/>
+    </row>
+    <row r="65533" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F65533" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="G65532" s="27"/>
+      <c r="G65533" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3713,22 +3832,22 @@
   <dimension ref="A4:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -3737,7 +3856,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
@@ -3745,27 +3864,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>

</xml_diff>

<commit_message>
corrected demand to be used by both 2nd and 3th day
</commit_message>
<xml_diff>
--- a/VT_SHR_SUP_V01.xlsx
+++ b/VT_SHR_SUP_V01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Najub\TIMES-Shire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mikkel\TIMES-DK\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901"/>
+    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -2093,7 +2093,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
@@ -2951,23 +2951,23 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2976,13 +2976,13 @@
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="6" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
         <v>42</v>
       </c>
@@ -2995,7 +2995,7 @@
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="36" t="s">
         <v>14</v>
       </c>
@@ -3008,7 +3008,7 @@
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="37" t="s">
         <v>7</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="40" t="s">
         <v>47</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="42" t="s">
         <v>58</v>
       </c>
@@ -3085,7 +3085,7 @@
       <c r="I10" s="42"/>
       <c r="J10" s="42"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
@@ -3102,7 +3102,7 @@
       <c r="I11" s="42"/>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
       <c r="D12" s="42" t="s">
@@ -3119,7 +3119,7 @@
       <c r="I12" s="42"/>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42" t="s">
@@ -3136,7 +3136,7 @@
       <c r="I13" s="42"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
       <c r="D14" s="42" t="s">
@@ -3153,7 +3153,7 @@
       <c r="I14" s="42"/>
       <c r="J14" s="42"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="s">
@@ -3170,7 +3170,7 @@
       <c r="I15" s="42"/>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
       <c r="D16" s="42" t="s">
@@ -3187,7 +3187,7 @@
       <c r="I16" s="42"/>
       <c r="J16" s="42"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
       <c r="D17" s="55" t="s">
@@ -3204,7 +3204,7 @@
       <c r="I17" s="42"/>
       <c r="J17" s="42"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
@@ -3221,7 +3221,7 @@
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="42"/>
       <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
@@ -3238,7 +3238,7 @@
       <c r="I19" s="42"/>
       <c r="J19" s="42"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="42"/>
       <c r="C20" s="43"/>
       <c r="D20" s="55" t="s">
@@ -3255,7 +3255,7 @@
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="42" t="s">
         <v>63</v>
       </c>
@@ -3274,7 +3274,7 @@
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>58</v>
       </c>
@@ -3293,7 +3293,7 @@
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
       <c r="D23" s="43" t="s">
@@ -3329,32 +3329,32 @@
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="33" t="s">
         <v>43</v>
@@ -3368,7 +3368,7 @@
       <c r="I5" s="44"/>
       <c r="J5" s="44"/>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="36" t="s">
         <v>16</v>
       </c>
@@ -3381,7 +3381,7 @@
       <c r="I6" s="44"/>
       <c r="J6" s="44"/>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="38" t="s">
         <v>11</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="41" t="s">
         <v>48</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="42" t="s">
         <v>68</v>
       </c>
@@ -3460,7 +3460,7 @@
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="42" t="s">
         <v>70</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
@@ -3500,7 +3500,7 @@
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
       <c r="C12" s="43"/>
       <c r="D12" s="42" t="s">
@@ -3519,7 +3519,7 @@
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="42"/>
       <c r="C13" s="43"/>
       <c r="D13" s="55" t="s">
@@ -3538,7 +3538,7 @@
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
       <c r="D14" s="42" t="s">
@@ -3557,7 +3557,7 @@
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="str">
@@ -3578,7 +3578,7 @@
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
       <c r="D16" s="42" t="str">
@@ -3599,7 +3599,7 @@
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="42" t="s">
         <v>65</v>
       </c>
@@ -3620,7 +3620,7 @@
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
@@ -3639,7 +3639,7 @@
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
@@ -3658,7 +3658,7 @@
       <c r="I19" s="43"/>
       <c r="J19" s="43"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
       <c r="D20" s="42" t="s">
@@ -3677,7 +3677,7 @@
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="42" t="s">
@@ -3696,7 +3696,7 @@
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
       <c r="D22" s="42" t="s">
@@ -3715,7 +3715,7 @@
       <c r="I22" s="42"/>
       <c r="J22" s="42"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42" t="s">
@@ -3734,7 +3734,7 @@
       <c r="I23" s="42"/>
       <c r="J23" s="42"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="42"/>
       <c r="C24" s="42"/>
       <c r="D24" s="55" t="s">
@@ -3753,7 +3753,7 @@
       <c r="I24" s="42"/>
       <c r="J24" s="42"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="42"/>
       <c r="C25" s="42"/>
       <c r="D25" s="42" t="s">
@@ -3772,7 +3772,7 @@
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="42"/>
       <c r="C26" s="42"/>
       <c r="D26" s="42" t="str">
@@ -3793,7 +3793,7 @@
       <c r="I26" s="42"/>
       <c r="J26" s="42"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="42"/>
       <c r="C27" s="42"/>
       <c r="D27" s="42" t="str">
@@ -3831,23 +3831,23 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.88671875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.85546875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="15" customWidth="1"/>
     <col min="11" max="50" width="6" style="15" customWidth="1"/>
-    <col min="51" max="51" width="9.109375" style="15"/>
+    <col min="51" max="51" width="9.140625" style="15"/>
     <col min="52" max="52" width="12" style="15" customWidth="1"/>
-    <col min="53" max="16384" width="9.109375" style="15"/>
+    <col min="53" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>56</v>
       </c>
@@ -3855,14 +3855,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2"/>
       <c r="I2"/>
       <c r="J2" s="30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I4" s="30" t="s">
         <v>78</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
@@ -3894,7 +3894,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6"/>
@@ -3905,7 +3905,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -3916,7 +3916,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24"/>
       <c r="B9" s="45" t="s">
         <v>49</v>
@@ -3989,7 +3989,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="46" t="s">
         <v>80</v>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="M10" s="47"/>
     </row>
-    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25"/>
       <c r="B11" s="26" t="str">
         <f>SEC_Processes!D9</f>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="M11" s="48"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="25"/>
       <c r="B12" s="26" t="str">
         <f>SEC_Processes!D17</f>
@@ -4092,7 +4092,7 @@
       </c>
       <c r="M12" s="48"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="25"/>
       <c r="B13" s="26" t="str">
         <f>SEC_Processes!D18</f>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="M13" s="48"/>
     </row>
-    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25"/>
       <c r="B14" s="26" t="str">
         <f>SEC_Processes!D19</f>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="M14" s="48"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="25"/>
       <c r="B15" s="26" t="str">
         <f>SEC_Processes!D20</f>
@@ -4193,7 +4193,7 @@
       </c>
       <c r="M15" s="48"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="26" t="str">
         <f>SEC_Processes!D21</f>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="M16" s="48"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="26" t="str">
         <f>SEC_Processes!D22</f>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="M17" s="48"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="26" t="str">
         <f>SEC_Processes!D23</f>
@@ -4292,7 +4292,7 @@
       </c>
       <c r="M18" s="48"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="26" t="str">
         <f>SEC_Processes!D24</f>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="M19" s="48"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="26" t="str">
         <f>SEC_Processes!D25</f>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="M20" s="48"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="26" t="s">
         <v>128</v>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="M21" s="48"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="56" t="s">
         <v>168</v>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="M22" s="48"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="26" t="str">
         <f>SEC_Processes!D10</f>
@@ -4464,7 +4464,7 @@
       </c>
       <c r="M23" s="48"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" s="26" t="str">
         <f>SEC_Processes!D11</f>
         <v>EXPNGA</v>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="M24" s="48"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="str">
         <f>SEC_Processes!D12</f>
         <v>EXPDSL</v>
@@ -4532,7 +4532,7 @@
       </c>
       <c r="M25" s="48"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" s="26" t="str">
         <f>SEC_Processes!D13</f>
         <v>EXPWCH</v>
@@ -4567,7 +4567,7 @@
       </c>
       <c r="M26" s="48"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="26" t="str">
         <f>SEC_Processes!D14</f>
         <v>EXPSTR</v>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="M27" s="48"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" s="26" t="s">
         <v>130</v>
       </c>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="M28" s="48"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
         <v>170</v>
       </c>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="M29" s="48"/>
     </row>
-    <row r="65533" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="65533" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F65533" s="27" t="s">
         <v>85</v>
       </c>
@@ -4687,19 +4687,19 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -4708,7 +4708,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
@@ -4716,27 +4716,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
@@ -4752,29 +4752,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="49" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="2:10" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="51" t="s">
         <v>0</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>138</v>
       </c>
@@ -4796,28 +4796,28 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="E7">
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="E8">
         <v>4000</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="38" t="s">
         <v>1</v>
       </c>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="J14" s="38"/>
     </row>
-    <row r="15" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="41" t="s">
         <v>49</v>
       </c>
@@ -4871,7 +4871,7 @@
       </c>
       <c r="J15" s="41"/>
     </row>
-    <row r="16" spans="2:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="46" t="s">
         <v>80</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="43" t="s">
         <v>151</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="43" t="s">
         <v>149</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="43" t="s">
         <v>150</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="36" t="s">
         <v>16</v>
       </c>
@@ -4976,7 +4976,7 @@
       <c r="I25" s="44"/>
       <c r="J25" s="44"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="38" t="s">
         <v>11</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="41" t="s">
         <v>48</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="43" t="s">
         <v>161</v>
       </c>
@@ -5053,7 +5053,7 @@
       <c r="I28" s="54"/>
       <c r="J28" s="54"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" s="43"/>
       <c r="C29" s="43"/>
       <c r="D29" s="43" t="s">
@@ -5070,7 +5070,7 @@
       <c r="I29" s="54"/>
       <c r="J29" s="54"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
       <c r="D30" s="43" t="s">
@@ -5087,7 +5087,7 @@
       <c r="I30" s="54"/>
       <c r="J30" s="54"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32" s="36" t="s">
         <v>14</v>
       </c>
@@ -5100,7 +5100,7 @@
       <c r="I32" s="35"/>
       <c r="J32" s="35"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="37" t="s">
         <v>7</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="40" t="s">
         <v>47</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="43" t="s">
         <v>58</v>
       </c>
@@ -5177,7 +5177,7 @@
       <c r="I35" s="43"/>
       <c r="J35" s="43"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
       <c r="D36" s="43" t="s">
@@ -5194,7 +5194,7 @@
       <c r="I36" s="43"/>
       <c r="J36" s="43"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="43"/>
       <c r="C37" s="43"/>
       <c r="D37" s="43" t="s">

</xml_diff>

<commit_message>
Demand naming adjusted (small inconsistency was found in the Day-2 branch)
</commit_message>
<xml_diff>
--- a/VT_SHR_SUP_V01.xlsx
+++ b/VT_SHR_SUP_V01.xlsx
@@ -4750,7 +4750,7 @@
   <dimension ref="B4:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4795,7 +4795,7 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="E7">
         <v>2000</v>
@@ -4803,7 +4803,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="E8">
         <v>4000</v>

</xml_diff>

<commit_message>
Deleted demands from the SUP file
</commit_message>
<xml_diff>
--- a/VT_SHR_SUP_V01.xlsx
+++ b/VT_SHR_SUP_V01.xlsx
@@ -5,26 +5,25 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Najub\TIMES-Shire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stpet\Git models\TIMES-SHIRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901" activeTab="4"/>
+    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
     <sheet name="ProcessCharac_Horizontal" sheetId="131" r:id="rId2"/>
     <sheet name="SEC_Processes" sheetId="127" r:id="rId3"/>
     <sheet name="EmissionTable" sheetId="126" r:id="rId4"/>
-    <sheet name="Demand" sheetId="132" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -821,758 +820,8 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Maurizio Gargiulo</author>
-    <author>Amit Kanudia</author>
-    <author>Gary Goldstein</author>
-  </authors>
-  <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Total DKE demand
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H26" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Allowed TsLvl
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ANNUAL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Annual level)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>SEASON</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Seasonal level)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>WEEKLY</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Weekly level)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DAYNITE</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (day and night level)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I26" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Amit Kanudia:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Needed only when one wants to override the VEDA default assignment
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J26" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allowed Vintage</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-NO</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (if empty by default mean </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>NO</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-YES</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B27" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Sets declarations are </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>inherited. 
-Allowed Process Sets</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-ELE </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Thermal Electric Power Plant)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-CHP </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Combined Heat and Power)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-STGTSS </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Pump Storage)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-STGIPS</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Pump Storage IP)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-PRE </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Genric Process/Technology)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-DMD</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Demand Device)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-IMP </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">(Import)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>EXP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Export)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-MIN </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Mining Process)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-RNW </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Renewable Technology)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-HPL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Heating Plant)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B33" authorId="2" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Csets declarations are inherited until the next one is encountered.
-Allowed Cset:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>NRG</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Energy)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ENV</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Emission)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DEM</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Demand)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MAT</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Material)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>FIN</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Financial)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G33" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Amit Kanudia:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-LO for PRODUCTION &gt;= CONSUMPTION (Default)
-FX for PRODUCTION = CONSUMPTION
-UP for PRODUCTION &lt;= CONSUMPTION</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allowed CTSLvl</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-SEASON</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Seasonal level)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-WEEKLY</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Weekly level)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-DAYNITE</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (day and night level)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allowed PeakTS</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-ANNUAL </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(to generate Peak Equation for all the TimeSlices)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-User TS </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(to generate Peak Equation for a single TS)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Allowed Ctype
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ELC</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Electricity)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="147">
   <si>
     <t>CommName</t>
   </si>
@@ -1983,78 +1232,6 @@
   </si>
   <si>
     <t>Gasoline</t>
-  </si>
-  <si>
-    <t>*Description</t>
-  </si>
-  <si>
-    <t>FUEL</t>
-  </si>
-  <si>
-    <t>DEMAND</t>
-  </si>
-  <si>
-    <t>EFF</t>
-  </si>
-  <si>
-    <t>NCAP_COST</t>
-  </si>
-  <si>
-    <t>NCAP_TLIFE</t>
-  </si>
-  <si>
-    <t>Technology description</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Effeciency</t>
-  </si>
-  <si>
-    <t>Lifetime of Process</t>
-  </si>
-  <si>
-    <t>Years</t>
-  </si>
-  <si>
-    <t>Capital Investment Cost</t>
-  </si>
-  <si>
-    <t>FCELCC</t>
-  </si>
-  <si>
-    <t>FCHET</t>
-  </si>
-  <si>
-    <t>FCFUEL</t>
-  </si>
-  <si>
-    <t>Final consumption Fuel</t>
-  </si>
-  <si>
-    <t>Final consumption Electrciity</t>
-  </si>
-  <si>
-    <t>Final Consumption Heat</t>
-  </si>
-  <si>
-    <t>CRD, DSL, NGA</t>
-  </si>
-  <si>
-    <t>HEAT</t>
-  </si>
-  <si>
-    <t>POWER</t>
-  </si>
-  <si>
-    <t>MEUR2011</t>
-  </si>
-  <si>
-    <t>FUELS</t>
-  </si>
-  <si>
-    <t>PRE</t>
   </si>
   <si>
     <t>WCH</t>
@@ -2090,11 +1267,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2207,13 +1384,6 @@
       <sz val="20"/>
       <color theme="2" tint="-9.9978637043366805E-2"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2334,7 +1504,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2418,22 +1588,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -2952,19 +2106,19 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2973,13 +2127,13 @@
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="6" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
         <v>42</v>
       </c>
@@ -2992,7 +2146,7 @@
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="36" t="s">
         <v>14</v>
       </c>
@@ -3005,7 +2159,7 @@
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="37" t="s">
         <v>7</v>
       </c>
@@ -3034,7 +2188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="40" t="s">
         <v>47</v>
       </c>
@@ -3063,7 +2217,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="42" t="s">
         <v>58</v>
       </c>
@@ -3082,7 +2236,7 @@
       <c r="I10" s="42"/>
       <c r="J10" s="42"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
@@ -3099,7 +2253,7 @@
       <c r="I11" s="42"/>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
       <c r="D12" s="42" t="s">
@@ -3116,7 +2270,7 @@
       <c r="I12" s="42"/>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42" t="s">
@@ -3133,7 +2287,7 @@
       <c r="I13" s="42"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
       <c r="D14" s="42" t="s">
@@ -3150,7 +2304,7 @@
       <c r="I14" s="42"/>
       <c r="J14" s="42"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="s">
@@ -3167,7 +2321,7 @@
       <c r="I15" s="42"/>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
       <c r="D16" s="42" t="s">
@@ -3184,11 +2338,11 @@
       <c r="I16" s="42"/>
       <c r="J16" s="42"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
-      <c r="D17" s="55" t="s">
-        <v>161</v>
+      <c r="D17" s="49" t="s">
+        <v>137</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>94</v>
@@ -3201,7 +2355,7 @@
       <c r="I17" s="42"/>
       <c r="J17" s="42"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
@@ -3218,7 +2372,7 @@
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="42"/>
       <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
@@ -3235,16 +2389,16 @@
       <c r="I19" s="42"/>
       <c r="J19" s="42"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="42"/>
       <c r="C20" s="43"/>
-      <c r="D20" s="55" t="s">
-        <v>165</v>
-      </c>
-      <c r="E20" s="55" t="s">
-        <v>166</v>
-      </c>
-      <c r="F20" s="55" t="s">
+      <c r="D20" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="49" t="s">
         <v>59</v>
       </c>
       <c r="G20" s="42"/>
@@ -3252,7 +2406,7 @@
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="42" t="s">
         <v>63</v>
       </c>
@@ -3271,7 +2425,7 @@
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>58</v>
       </c>
@@ -3290,7 +2444,7 @@
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
       <c r="D23" s="43" t="s">
@@ -3305,8 +2459,8 @@
       <c r="G23" s="43"/>
       <c r="H23" s="43"/>
       <c r="I23" s="43"/>
-      <c r="J23" s="55" t="s">
-        <v>164</v>
+      <c r="J23" s="49" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3326,23 +2480,23 @@
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.88671875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.85546875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="15" customWidth="1"/>
     <col min="11" max="50" width="6" style="15" customWidth="1"/>
-    <col min="51" max="51" width="9.109375" style="15"/>
+    <col min="51" max="51" width="9.140625" style="15"/>
     <col min="52" max="52" width="12" style="15" customWidth="1"/>
-    <col min="53" max="16384" width="9.109375" style="15"/>
+    <col min="53" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>56</v>
       </c>
@@ -3350,14 +2504,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2"/>
       <c r="I2"/>
       <c r="J2" s="30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
@@ -3368,7 +2522,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I4" s="30" t="s">
         <v>78</v>
       </c>
@@ -3376,7 +2530,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
@@ -3389,7 +2543,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6"/>
@@ -3400,7 +2554,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -3411,7 +2565,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
@@ -3449,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24"/>
       <c r="B9" s="45" t="s">
         <v>49</v>
@@ -3484,7 +2638,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="46" t="s">
         <v>80</v>
@@ -3509,7 +2663,7 @@
       </c>
       <c r="M10" s="47"/>
     </row>
-    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25"/>
       <c r="B11" s="26" t="str">
         <f>SEC_Processes!D9</f>
@@ -3550,7 +2704,7 @@
       </c>
       <c r="M11" s="48"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="25"/>
       <c r="B12" s="26" t="str">
         <f>SEC_Processes!D17</f>
@@ -3587,7 +2741,7 @@
       </c>
       <c r="M12" s="48"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="25"/>
       <c r="B13" s="26" t="str">
         <f>SEC_Processes!D18</f>
@@ -3622,7 +2776,7 @@
       </c>
       <c r="M13" s="48"/>
     </row>
-    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25"/>
       <c r="B14" s="26" t="str">
         <f>SEC_Processes!D19</f>
@@ -3655,7 +2809,7 @@
       </c>
       <c r="M14" s="48"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="25"/>
       <c r="B15" s="26" t="str">
         <f>SEC_Processes!D20</f>
@@ -3688,7 +2842,7 @@
       </c>
       <c r="M15" s="48"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="26" t="str">
         <f>SEC_Processes!D21</f>
@@ -3721,7 +2875,7 @@
       </c>
       <c r="M16" s="48"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="26" t="str">
         <f>SEC_Processes!D22</f>
@@ -3754,7 +2908,7 @@
       </c>
       <c r="M17" s="48"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="26" t="str">
         <f>SEC_Processes!D23</f>
@@ -3787,7 +2941,7 @@
       </c>
       <c r="M18" s="48"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="26" t="str">
         <f>SEC_Processes!D24</f>
@@ -3821,7 +2975,7 @@
       </c>
       <c r="M19" s="48"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="26" t="str">
         <f>SEC_Processes!D25</f>
@@ -3854,7 +3008,7 @@
       </c>
       <c r="M20" s="48"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="26" t="s">
         <v>128</v>
@@ -3887,17 +3041,17 @@
       </c>
       <c r="M21" s="48"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
-      <c r="B22" s="56" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" s="56" t="s">
-        <v>168</v>
+      <c r="B22" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>144</v>
       </c>
       <c r="D22" s="26"/>
-      <c r="E22" s="56" t="s">
-        <v>165</v>
+      <c r="E22" s="50" t="s">
+        <v>141</v>
       </c>
       <c r="F22" s="27" t="s">
         <v>74</v>
@@ -3918,7 +3072,7 @@
       </c>
       <c r="M22" s="48"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="26" t="str">
         <f>SEC_Processes!D10</f>
@@ -3959,7 +3113,7 @@
       </c>
       <c r="M23" s="48"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" s="26" t="str">
         <f>SEC_Processes!D11</f>
         <v>EXPNGA</v>
@@ -3993,7 +3147,7 @@
       </c>
       <c r="M24" s="48"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="str">
         <f>SEC_Processes!D12</f>
         <v>EXPDSL</v>
@@ -4027,7 +3181,7 @@
       </c>
       <c r="M25" s="48"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" s="26" t="str">
         <f>SEC_Processes!D13</f>
         <v>EXPWCH</v>
@@ -4062,7 +3216,7 @@
       </c>
       <c r="M26" s="48"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="26" t="str">
         <f>SEC_Processes!D14</f>
         <v>EXPSTR</v>
@@ -4096,7 +3250,7 @@
       </c>
       <c r="M27" s="48"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" s="26" t="s">
         <v>130</v>
       </c>
@@ -4128,15 +3282,15 @@
       </c>
       <c r="M28" s="48"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="27" t="s">
@@ -4160,7 +3314,7 @@
       </c>
       <c r="M29" s="48"/>
     </row>
-    <row r="65533" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="65533" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F65533" s="27" t="s">
         <v>85</v>
       </c>
@@ -4182,32 +3336,32 @@
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="33" t="s">
         <v>43</v>
@@ -4221,7 +3375,7 @@
       <c r="I5" s="44"/>
       <c r="J5" s="44"/>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="36" t="s">
         <v>16</v>
       </c>
@@ -4234,7 +3388,7 @@
       <c r="I6" s="44"/>
       <c r="J6" s="44"/>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="38" t="s">
         <v>11</v>
       </c>
@@ -4263,7 +3417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="41" t="s">
         <v>48</v>
       </c>
@@ -4292,7 +3446,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="42" t="s">
         <v>68</v>
       </c>
@@ -4313,7 +3467,7 @@
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="42" t="s">
         <v>70</v>
       </c>
@@ -4334,7 +3488,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
@@ -4353,7 +3507,7 @@
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
       <c r="C12" s="43"/>
       <c r="D12" s="42" t="s">
@@ -4372,11 +3526,11 @@
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="42"/>
       <c r="C13" s="43"/>
-      <c r="D13" s="55" t="s">
-        <v>162</v>
+      <c r="D13" s="49" t="s">
+        <v>138</v>
       </c>
       <c r="E13" s="42" t="s">
         <v>103</v>
@@ -4391,7 +3545,7 @@
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
       <c r="D14" s="42" t="s">
@@ -4410,7 +3564,7 @@
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="str">
@@ -4431,7 +3585,7 @@
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
       <c r="D16" s="42" t="str">
@@ -4442,7 +3596,7 @@
         <f>ProcessCharac_Horizontal!C29</f>
         <v>Export Uranium</v>
       </c>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="49" t="s">
         <v>59</v>
       </c>
       <c r="G16" s="42" t="s">
@@ -4452,7 +3606,7 @@
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="42" t="s">
         <v>65</v>
       </c>
@@ -4473,7 +3627,7 @@
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
@@ -4492,7 +3646,7 @@
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
@@ -4511,7 +3665,7 @@
       <c r="I19" s="43"/>
       <c r="J19" s="43"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
       <c r="D20" s="42" t="s">
@@ -4530,7 +3684,7 @@
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="42" t="s">
@@ -4549,7 +3703,7 @@
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
       <c r="D22" s="42" t="s">
@@ -4568,7 +3722,7 @@
       <c r="I22" s="42"/>
       <c r="J22" s="42"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42" t="s">
@@ -4587,11 +3741,11 @@
       <c r="I23" s="42"/>
       <c r="J23" s="42"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="42"/>
       <c r="C24" s="42"/>
-      <c r="D24" s="55" t="s">
-        <v>163</v>
+      <c r="D24" s="49" t="s">
+        <v>139</v>
       </c>
       <c r="E24" s="42" t="s">
         <v>115</v>
@@ -4606,7 +3760,7 @@
       <c r="I24" s="42"/>
       <c r="J24" s="42"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="42"/>
       <c r="C25" s="42"/>
       <c r="D25" s="42" t="s">
@@ -4625,7 +3779,7 @@
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="42"/>
       <c r="C26" s="42"/>
       <c r="D26" s="42" t="str">
@@ -4646,7 +3800,7 @@
       <c r="I26" s="42"/>
       <c r="J26" s="42"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="42"/>
       <c r="C27" s="42"/>
       <c r="D27" s="42" t="str">
@@ -4680,23 +3834,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -4705,7 +3859,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
@@ -4713,27 +3867,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
@@ -4743,473 +3897,4 @@
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:J37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="50"/>
-    </row>
-    <row r="5" spans="2:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B5" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="51" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>157</v>
-      </c>
-      <c r="E7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E8">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="I14" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="J14" s="38"/>
-    </row>
-    <row r="15" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="H15" s="53" t="s">
-        <v>148</v>
-      </c>
-      <c r="I15" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="J15" s="41"/>
-    </row>
-    <row r="16" spans="2:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="J16" s="46" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="G17" s="54">
-        <v>1</v>
-      </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="D18" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="G18" s="54">
-        <v>1</v>
-      </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="F19" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="G19" s="54">
-        <v>1</v>
-      </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="J27" s="41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="s">
-        <v>160</v>
-      </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G28" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="I33" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="J33" s="39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="G34" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="H34" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="I34" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="J34" s="40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="E35" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="F35" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="E36" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="F36" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="E37" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="F37" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed the text for WPE to wood pellets (from wood chips)
</commit_message>
<xml_diff>
--- a/VT_SHR_SUP_V01.xlsx
+++ b/VT_SHR_SUP_V01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Najub\TIMES-Shire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stpet\Git models\TIMES-SHIRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901"/>
+    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1105,9 +1105,6 @@
     <t>Solar</t>
   </si>
   <si>
-    <t>Woodchips</t>
-  </si>
-  <si>
     <t>STR</t>
   </si>
   <si>
@@ -1132,9 +1129,6 @@
     <t>Export Diesel</t>
   </si>
   <si>
-    <t>Export Woodchips</t>
-  </si>
-  <si>
     <t>EXPSTR</t>
   </si>
   <si>
@@ -1168,9 +1162,6 @@
     <t>Import Solar</t>
   </si>
   <si>
-    <t>Import Woodchips</t>
-  </si>
-  <si>
     <t>Import Straw</t>
   </si>
   <si>
@@ -1262,12 +1253,21 @@
   </si>
   <si>
     <t>ELC</t>
+  </si>
+  <si>
+    <t>Export Wood pellets</t>
+  </si>
+  <si>
+    <t>Import Wood pellets</t>
+  </si>
+  <si>
+    <t>Wood pellets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
@@ -2100,22 +2100,22 @@
   <dimension ref="B1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2124,13 +2124,13 @@
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="6" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
         <v>42</v>
       </c>
@@ -2143,7 +2143,7 @@
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="36" t="s">
         <v>14</v>
       </c>
@@ -2156,7 +2156,7 @@
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="37" t="s">
         <v>7</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="40" t="s">
         <v>47</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="42" t="s">
         <v>58</v>
       </c>
@@ -2233,7 +2233,7 @@
       <c r="I10" s="42"/>
       <c r="J10" s="42"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
@@ -2250,7 +2250,7 @@
       <c r="I11" s="42"/>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
       <c r="D12" s="42" t="s">
@@ -2267,14 +2267,14 @@
       <c r="I12" s="42"/>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F13" s="42" t="s">
         <v>59</v>
@@ -2284,7 +2284,7 @@
       <c r="I13" s="42"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
       <c r="D14" s="42" t="s">
@@ -2301,7 +2301,7 @@
       <c r="I14" s="42"/>
       <c r="J14" s="42"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="s">
@@ -2318,7 +2318,7 @@
       <c r="I15" s="42"/>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
       <c r="D16" s="42" t="s">
@@ -2335,14 +2335,14 @@
       <c r="I16" s="42"/>
       <c r="J16" s="42"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
       <c r="D17" s="42" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>59</v>
@@ -2352,14 +2352,14 @@
       <c r="I17" s="42"/>
       <c r="J17" s="42"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="42" t="s">
         <v>95</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>96</v>
       </c>
       <c r="F18" s="42" t="s">
         <v>59</v>
@@ -2369,14 +2369,14 @@
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="42"/>
       <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F19" s="42" t="s">
         <v>59</v>
@@ -2386,14 +2386,14 @@
       <c r="I19" s="42"/>
       <c r="J19" s="42"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="42"/>
       <c r="C20" s="43"/>
       <c r="D20" s="42" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>59</v>
@@ -2403,7 +2403,7 @@
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="42" t="s">
         <v>63</v>
       </c>
@@ -2422,16 +2422,16 @@
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>58</v>
       </c>
       <c r="C22" s="43"/>
       <c r="D22" s="43" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F22" s="43" t="s">
         <v>59</v>
@@ -2441,14 +2441,14 @@
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
       <c r="D23" s="43" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F23" s="43" t="s">
         <v>59</v>
@@ -2457,7 +2457,7 @@
       <c r="H23" s="43"/>
       <c r="I23" s="43"/>
       <c r="J23" s="43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2474,35 +2474,35 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="33" t="s">
         <v>43</v>
@@ -2516,7 +2516,7 @@
       <c r="I5" s="44"/>
       <c r="J5" s="44"/>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="36" t="s">
         <v>16</v>
       </c>
@@ -2529,7 +2529,7 @@
       <c r="I6" s="44"/>
       <c r="J6" s="44"/>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="38" t="s">
         <v>11</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="41" t="s">
         <v>48</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="42" t="s">
         <v>68</v>
       </c>
@@ -2596,19 +2596,19 @@
         <v>69</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G9" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="42" t="s">
         <v>70</v>
       </c>
@@ -2617,95 +2617,95 @@
         <v>71</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F10" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H10" s="43"/>
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
       <c r="D11" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="42" t="s">
         <v>97</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>98</v>
       </c>
       <c r="F11" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H11" s="43"/>
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
       <c r="C12" s="43"/>
       <c r="D12" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="42" t="s">
         <v>101</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>102</v>
       </c>
       <c r="F12" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H12" s="43"/>
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="42"/>
       <c r="C13" s="43"/>
       <c r="D13" s="42" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="F13" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H13" s="43"/>
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
       <c r="D14" s="42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F14" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G14" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H14" s="43"/>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="42" t="str">
@@ -2720,13 +2720,13 @@
         <v>59</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H15" s="43"/>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
       <c r="D16" s="42" t="str">
@@ -2741,13 +2741,13 @@
         <v>59</v>
       </c>
       <c r="G16" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H16" s="43"/>
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="42" t="s">
         <v>65</v>
       </c>
@@ -2756,171 +2756,171 @@
         <v>66</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G17" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H17" s="43"/>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="42" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F18" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G18" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H18" s="43"/>
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
       <c r="D19" s="42" t="s">
         <v>67</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F19" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H19" s="43"/>
       <c r="I19" s="43"/>
       <c r="J19" s="43"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
       <c r="D20" s="42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H20" s="42"/>
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F21" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G21" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H21" s="42"/>
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
       <c r="D22" s="42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F22" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G22" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="42"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F23" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H23" s="42"/>
       <c r="I23" s="42"/>
       <c r="J23" s="42"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="42"/>
       <c r="C24" s="42"/>
       <c r="D24" s="42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="F24" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="42"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="42"/>
       <c r="C25" s="42"/>
       <c r="D25" s="42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F25" s="42" t="s">
         <v>59</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="42"/>
       <c r="C26" s="42"/>
       <c r="D26" s="42" t="str">
@@ -2935,13 +2935,13 @@
         <v>59</v>
       </c>
       <c r="G26" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
       <c r="J26" s="42"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="42"/>
       <c r="C27" s="42"/>
       <c r="D27" s="42" t="str">
@@ -2956,7 +2956,7 @@
         <v>59</v>
       </c>
       <c r="G27" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H27" s="42"/>
       <c r="I27" s="42"/>
@@ -2976,26 +2976,26 @@
   <dimension ref="A1:M65533"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.88671875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.85546875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="15" customWidth="1"/>
     <col min="11" max="50" width="6" style="15" customWidth="1"/>
-    <col min="51" max="51" width="9.109375" style="15"/>
+    <col min="51" max="51" width="9.140625" style="15"/>
     <col min="52" max="52" width="12" style="15" customWidth="1"/>
-    <col min="53" max="16384" width="9.109375" style="15"/>
+    <col min="53" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>56</v>
       </c>
@@ -3003,14 +3003,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2"/>
       <c r="I2"/>
       <c r="J2" s="30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I4" s="30" t="s">
         <v>78</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
@@ -3042,7 +3042,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6"/>
@@ -3053,7 +3053,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -3064,7 +3064,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>73</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H8" s="23" t="s">
         <v>45</v>
@@ -3102,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="38.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24"/>
       <c r="B9" s="45" t="s">
         <v>49</v>
@@ -3137,7 +3137,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="46" t="s">
         <v>80</v>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="M10" s="47"/>
     </row>
-    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25"/>
       <c r="B11" s="26" t="str">
         <f>SEC_Processes!D9</f>
@@ -3180,7 +3180,7 @@
         <v>74</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>79</v>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="M11" s="48"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="25"/>
       <c r="B12" s="26" t="str">
         <f>SEC_Processes!D17</f>
@@ -3221,7 +3221,7 @@
         <v>74</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>79</v>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="M12" s="48"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="25"/>
       <c r="B13" s="26" t="str">
         <f>SEC_Processes!D18</f>
@@ -3252,13 +3252,13 @@
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>74</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>79</v>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="M13" s="48"/>
     </row>
-    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25"/>
       <c r="B14" s="26" t="str">
         <f>SEC_Processes!D19</f>
@@ -3293,7 +3293,7 @@
         <v>74</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H14" s="28" t="s">
         <v>79</v>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="M14" s="48"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="25"/>
       <c r="B15" s="26" t="str">
         <f>SEC_Processes!D20</f>
@@ -3326,7 +3326,7 @@
         <v>74</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H15" s="28" t="s">
         <v>79</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="M15" s="48"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="26" t="str">
         <f>SEC_Processes!D21</f>
@@ -3359,7 +3359,7 @@
         <v>74</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>79</v>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="M16" s="48"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="26" t="str">
         <f>SEC_Processes!D22</f>
@@ -3392,7 +3392,7 @@
         <v>74</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H17" s="28" t="s">
         <v>79</v>
@@ -3407,7 +3407,7 @@
       </c>
       <c r="M17" s="48"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="26" t="str">
         <f>SEC_Processes!D23</f>
@@ -3425,7 +3425,7 @@
         <v>74</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H18" s="28" t="s">
         <v>79</v>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="M18" s="48"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="26" t="str">
         <f>SEC_Processes!D24</f>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="C19" s="26" t="str">
         <f>SEC_Processes!E24</f>
-        <v>Import Woodchips</v>
+        <v>Import Wood pellets</v>
       </c>
       <c r="D19" s="26"/>
       <c r="E19" s="26" t="str">
@@ -3459,7 +3459,7 @@
         <v>74</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H19" s="28" t="s">
         <v>79</v>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="M19" s="48"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="26" t="str">
         <f>SEC_Processes!D25</f>
@@ -3486,13 +3486,13 @@
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="27" t="s">
         <v>74</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>79</v>
@@ -3507,23 +3507,23 @@
       </c>
       <c r="M20" s="48"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F21" s="27" t="s">
         <v>74</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H21" s="28" t="s">
         <v>79</v>
@@ -3540,23 +3540,23 @@
       </c>
       <c r="M21" s="48"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F22" s="27" t="s">
         <v>74</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H22" s="28" t="s">
         <v>79</v>
@@ -3571,7 +3571,7 @@
       </c>
       <c r="M22" s="48"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="26" t="str">
         <f>SEC_Processes!D10</f>
@@ -3589,7 +3589,7 @@
         <v>74</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H23" s="28" t="s">
         <v>79</v>
@@ -3612,7 +3612,7 @@
       </c>
       <c r="M23" s="48"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" s="26" t="str">
         <f>SEC_Processes!D11</f>
         <v>EXPNGA</v>
@@ -3629,7 +3629,7 @@
         <v>74</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>79</v>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="M24" s="48"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="str">
         <f>SEC_Processes!D12</f>
         <v>EXPDSL</v>
@@ -3663,7 +3663,7 @@
         <v>74</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H25" s="28" t="s">
         <v>79</v>
@@ -3680,14 +3680,14 @@
       </c>
       <c r="M25" s="48"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" s="26" t="str">
         <f>SEC_Processes!D13</f>
         <v>EXPWPE</v>
       </c>
       <c r="C26" s="26" t="str">
         <f>SEC_Processes!E13</f>
-        <v>Export Woodchips</v>
+        <v>Export Wood pellets</v>
       </c>
       <c r="D26" s="26" t="str">
         <f>SEC_Comm!D17</f>
@@ -3698,7 +3698,7 @@
         <v>74</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H26" s="28" t="s">
         <v>79</v>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="M26" s="48"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="26" t="str">
         <f>SEC_Processes!D14</f>
         <v>EXPSTR</v>
@@ -3725,14 +3725,14 @@
         <v>Export Straw</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
         <v>74</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>79</v>
@@ -3749,22 +3749,22 @@
       </c>
       <c r="M27" s="48"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="27" t="s">
         <v>74</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H28" s="28" t="s">
         <v>79</v>
@@ -3781,22 +3781,22 @@
       </c>
       <c r="M28" s="48"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="27" t="s">
         <v>74</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H29" s="28" t="s">
         <v>79</v>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="M29" s="48"/>
     </row>
-    <row r="65533" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="65533" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F65533" s="27" t="s">
         <v>85</v>
       </c>
@@ -3835,19 +3835,19 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -3856,7 +3856,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
@@ -3864,27 +3864,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Corrected WIN; HYD to ELCC
</commit_message>
<xml_diff>
--- a/VT_SHR_SUP_V01.xlsx
+++ b/VT_SHR_SUP_V01.xlsx
@@ -1572,7 +1572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="171">
   <si>
     <t>CommName</t>
   </si>
@@ -2040,9 +2040,6 @@
   </si>
   <si>
     <t>CRD, DSL, NGA</t>
-  </si>
-  <si>
-    <t>WIN, HYD, SOL</t>
   </si>
   <si>
     <t>HEAT</t>
@@ -3191,7 +3188,7 @@
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
       <c r="D17" s="55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>94</v>
@@ -3242,10 +3239,10 @@
       <c r="B20" s="42"/>
       <c r="C20" s="43"/>
       <c r="D20" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="55" t="s">
         <v>166</v>
-      </c>
-      <c r="E20" s="55" t="s">
-        <v>167</v>
       </c>
       <c r="F20" s="55" t="s">
         <v>59</v>
@@ -3309,7 +3306,7 @@
       <c r="H23" s="43"/>
       <c r="I23" s="43"/>
       <c r="J23" s="55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3523,7 +3520,7 @@
       <c r="B13" s="42"/>
       <c r="C13" s="43"/>
       <c r="D13" s="55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E13" s="42" t="s">
         <v>103</v>
@@ -3738,7 +3735,7 @@
       <c r="B24" s="42"/>
       <c r="C24" s="42"/>
       <c r="D24" s="55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E24" s="42" t="s">
         <v>115</v>
@@ -4395,14 +4392,14 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="56" t="s">
         <v>168</v>
-      </c>
-      <c r="C22" s="56" t="s">
-        <v>169</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="56" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F22" s="27" t="s">
         <v>74</v>
@@ -4635,13 +4632,13 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="C29" s="26" t="s">
-        <v>171</v>
-      </c>
       <c r="D29" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="27" t="s">
@@ -4752,8 +4749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4798,7 +4795,7 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7">
         <v>2000</v>
@@ -4806,7 +4803,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E8">
         <v>4000</v>
@@ -4902,7 +4899,7 @@
         <v>138</v>
       </c>
       <c r="F17" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G17" s="54">
         <v>1</v>
@@ -4921,13 +4918,13 @@
         <v>153</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="E18" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="43" t="s">
         <v>158</v>
-      </c>
-      <c r="F18" s="43" t="s">
-        <v>159</v>
       </c>
       <c r="G18" s="54">
         <v>1</v>
@@ -4949,10 +4946,10 @@
         <v>122</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F19" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G19" s="54">
         <v>1</v>
@@ -5036,7 +5033,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C28" s="43"/>
       <c r="D28" s="43" t="s">
@@ -5164,7 +5161,7 @@
       </c>
       <c r="C35" s="43"/>
       <c r="D35" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E35" s="43" t="s">
         <v>124</v>
@@ -5181,7 +5178,7 @@
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
       <c r="D36" s="43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E36" s="43" t="s">
         <v>125</v>
@@ -5201,7 +5198,7 @@
         <v>138</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F37" s="43" t="s">
         <v>59</v>

</xml_diff>